<commit_message>
Add individual reading data for Oscar Andres Rincon Cardeño
</commit_message>
<xml_diff>
--- a/main/04_data_extraction/individual_reading.xlsx
+++ b/main/04_data_extraction/individual_reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\orincon\scoping-ml-wave-seismology\main\04_data_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6221BE29-0E7C-4D9A-B6AD-C7F3E0753CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5B146C-3884-47ED-9CC6-3612BA72FB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{115BB8D9-8B86-4726-97F8-E06477FD353D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{115BB8D9-8B86-4726-97F8-E06477FD353D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -1605,9 +1605,6 @@
     <t>Not specified. </t>
   </si>
   <si>
-    <t>Synthetic data. </t>
-  </si>
-  <si>
     <t> 2D.</t>
   </si>
   <si>
@@ -1649,12 +1646,15 @@
   <si>
     <t>Not reported.</t>
   </si>
+  <si>
+    <t>Synthetic data. Four datasets, of which three of them are used for seismic FWI, and one of which is for an EM inversion.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1876,6 +1876,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1887,12 +1893,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2332,7 +2332,7 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.59765625" customWidth="1"/>
     <col min="2" max="2" width="21.59765625" customWidth="1"/>
@@ -2349,49 +2349,49 @@
     <col min="15" max="16" width="18.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="88.5" customHeight="1">
+    <row r="1" spans="1:16" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="40"/>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38" t="s">
+      <c r="J1" s="40"/>
+      <c r="K1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="39" t="s">
+      <c r="L1" s="40"/>
+      <c r="M1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="25.5" customHeight="1">
+    <row r="2" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
@@ -2422,12 +2422,12 @@
       <c r="L2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="37"/>
-    </row>
-    <row r="3" spans="1:16" ht="21.75" customHeight="1">
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
@@ -2447,7 +2447,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15">
+    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -2467,7 +2467,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15">
+    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" ht="15">
+    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16" ht="15">
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:16" ht="15">
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -2547,7 +2547,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:16" ht="15">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:16" ht="15">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
@@ -2587,7 +2587,7 @@
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:16" ht="15">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:16" ht="15">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -2627,7 +2627,7 @@
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="1:16" ht="15">
+    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
@@ -2647,7 +2647,7 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:16" ht="15">
+    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
@@ -2667,7 +2667,7 @@
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:16" ht="15">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
@@ -2687,7 +2687,7 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:16" ht="15">
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>34</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="1:16" ht="15">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:16" ht="15">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="1:16" ht="15">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:16" ht="15">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:16" ht="15">
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
@@ -2807,7 +2807,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:16" ht="15">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>40</v>
       </c>
@@ -2827,7 +2827,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="1:16" ht="15">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>41</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="1:16" ht="15">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="1:16" ht="15">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>43</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="1:16" ht="15">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>44</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="1:16" ht="15">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>45</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="1:16" ht="15">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>46</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="1:16" ht="15">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>47</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="1:16" ht="15">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
@@ -2987,7 +2987,7 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="1:16" ht="15">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>49</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="1:16" ht="15">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>50</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="1:16" ht="15">
+    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>51</v>
       </c>
@@ -3047,7 +3047,7 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="1:16" ht="15">
+    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>52</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="1:16" ht="15">
+    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>53</v>
       </c>
@@ -3087,7 +3087,7 @@
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="1:16" ht="15">
+    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>54</v>
       </c>
@@ -3107,7 +3107,7 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="1:16" ht="15">
+    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>55</v>
       </c>
@@ -3127,7 +3127,7 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="1:16" ht="15">
+    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>56</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="1:16" ht="15">
+    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
@@ -3167,7 +3167,7 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="1:16" ht="15">
+    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>58</v>
       </c>
@@ -3187,7 +3187,7 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
     </row>
-    <row r="41" spans="1:16" ht="15">
+    <row r="41" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>59</v>
       </c>
@@ -3207,7 +3207,7 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row r="42" spans="1:16" ht="15">
+    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>60</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
     </row>
-    <row r="43" spans="1:16" ht="15">
+    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>61</v>
       </c>
@@ -3247,7 +3247,7 @@
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
     </row>
-    <row r="44" spans="1:16" ht="15">
+    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>62</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="45" spans="1:16" ht="15">
+    <row r="45" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>63</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
     </row>
-    <row r="46" spans="1:16" ht="15">
+    <row r="46" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>64</v>
       </c>
@@ -3332,7 +3332,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.09765625" bestFit="1" customWidth="1"/>
@@ -3349,7 +3349,7 @@
     <col min="15" max="15" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="78">
+    <row r="1" spans="1:15" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="409.6">
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15">
+    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -3458,7 +3458,7 @@
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
     </row>
-    <row r="4" spans="1:15" ht="409.6">
+    <row r="4" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>24</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15">
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>25</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="409.6">
+    <row r="7" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15">
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>27</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15">
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="409.6">
+    <row r="10" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15">
+    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>30</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15">
+    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>31</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="409.6">
+    <row r="13" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>32</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15">
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>33</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15">
+    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>34</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="409.6">
+    <row r="16" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>35</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15">
+    <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>36</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15">
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>37</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15">
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>38</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15">
+    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>39</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15">
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15">
+    <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>41</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15">
+    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>42</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15">
+    <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>43</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15">
+    <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>44</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15">
+    <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>45</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15">
+    <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>46</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15">
+    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>47</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15">
+    <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>48</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15">
+    <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>49</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15">
+    <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>50</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15">
+    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>51</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15">
+    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>52</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>53</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15">
+    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>54</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>55</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15">
+    <row r="37" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>56</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15">
+    <row r="38" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>57</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15">
+    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>58</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15">
+    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>59</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15">
+    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>60</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15">
+    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>61</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15">
+    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>62</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15">
+    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>63</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15">
+    <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>64</v>
       </c>
@@ -5441,11 +5441,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C33CE99-2E5D-4F6C-B637-1B3AEFE552A0}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.59765625" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.296875" style="21" customWidth="1"/>
@@ -5458,46 +5458,46 @@
     <col min="17" max="16384" width="9.09765625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="37"/>
+      <c r="G1" s="39"/>
       <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37" t="s">
+      <c r="J1" s="39"/>
+      <c r="K1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="40" t="s">
+      <c r="L1" s="39"/>
+      <c r="M1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="31.2">
+    <row r="2" spans="1:15" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
@@ -5528,11 +5528,11 @@
       <c r="L2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-    </row>
-    <row r="3" spans="1:15" ht="345">
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+    </row>
+    <row r="3" spans="1:15" ht="345" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>21</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="240">
+    <row r="4" spans="1:15" ht="240" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>22</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="270">
+    <row r="5" spans="1:15" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>23</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="255">
+    <row r="6" spans="1:15" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>24</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="330">
+    <row r="7" spans="1:15" ht="330" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>25</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="360">
+    <row r="8" spans="1:15" ht="360" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>26</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="270">
+    <row r="9" spans="1:15" ht="270" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>27</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="409.6">
+    <row r="10" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>28</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="270">
+    <row r="11" spans="1:15" ht="270" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>29</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="255">
+    <row r="12" spans="1:15" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>30</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="375">
+    <row r="13" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>31</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="409.6">
+    <row r="14" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>32</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="255">
+    <row r="15" spans="1:15" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>33</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="390">
+    <row r="16" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>34</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="45">
+    <row r="17" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>35</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="379.5" customHeight="1">
+    <row r="18" spans="1:16" ht="379.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>36</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="34" customFormat="1" ht="61.5" customHeight="1">
+    <row r="19" spans="1:16" s="34" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>37</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="409.6">
+    <row r="20" spans="1:16" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>38</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15">
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>39</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="60">
+    <row r="22" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>40</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="315">
+    <row r="23" spans="1:16" ht="315" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>41</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>42</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>43</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="330">
+    <row r="26" spans="1:16" ht="330" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>44</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>45</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="300">
+    <row r="28" spans="1:16" ht="300" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>46</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="34" customFormat="1" ht="409.6">
+    <row r="29" spans="1:16" s="34" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>47</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="315">
+    <row r="30" spans="1:16" ht="315" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>48</v>
       </c>
@@ -6819,34 +6819,34 @@
         <v>347</v>
       </c>
       <c r="H30" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="I30" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="J30" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="K30" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="K30" s="26" t="s">
+      <c r="L30" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="L30" s="26" t="s">
+      <c r="M30" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="M30" s="41" t="s">
+      <c r="N30" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="N30" s="25" t="s">
+      <c r="O30" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="P30" s="38" t="s">
         <v>354</v>
       </c>
-      <c r="O30" s="26" t="s">
-        <v>356</v>
-      </c>
-      <c r="P30" s="42" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="75">
+    </row>
+    <row r="31" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>49</v>
       </c>
@@ -6891,7 +6891,7 @@
       </c>
       <c r="O31" s="26"/>
     </row>
-    <row r="32" spans="1:16" ht="15">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>50</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="390">
+    <row r="33" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>51</v>
       </c>
@@ -6981,7 +6981,7 @@
       </c>
       <c r="O33" s="26"/>
     </row>
-    <row r="34" spans="1:15" ht="15">
+    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>52</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="75">
+    <row r="35" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>53</v>
       </c>
@@ -7071,7 +7071,7 @@
       </c>
       <c r="O35" s="26"/>
     </row>
-    <row r="36" spans="1:15" ht="15">
+    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>54</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="45">
+    <row r="37" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>55</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15">
+    <row r="38" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>56</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="90">
+    <row r="39" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>57</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15">
+    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>58</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="105">
+    <row r="41" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>59</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15">
+    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>60</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15">
+    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>61</v>
       </c>
@@ -7441,7 +7441,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15">
+    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>62</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15">
+    <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>63</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15">
+    <row r="46" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>64</v>
       </c>
@@ -7597,15 +7597,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010009048CEEA230F14796749F6DFD5F5263" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5105af4e7c1b0ed6cdb04338eaf51f7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="96457c7a-bdfc-427e-9d05-5faa5ab5244b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0baee1a300280ca08e7397f1756276d6" ns2:_="">
     <xsd:import namespace="96457c7a-bdfc-427e-9d05-5faa5ab5244b"/>
@@ -7749,6 +7740,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7756,14 +7756,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F2579D-323E-48EA-8FED-D372AFFF0A04}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75ADFBF6-8C74-4292-833E-68A026E87063}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7781,6 +7773,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F2579D-323E-48EA-8FED-D372AFFF0A04}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1160EB8C-E200-4916-A3B3-9BF8115D37F8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Add temporary files for data extraction: Dhara & Sen (2022) document and extracted reading data
</commit_message>
<xml_diff>
--- a/main/04_data_extraction/individual_reading.xlsx
+++ b/main/04_data_extraction/individual_reading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\orincon\scoping-ml-wave-seismology\main\04_data_extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5B146C-3884-47ED-9CC6-3612BA72FB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA3D48-EAB4-4754-BC97-D94457E4381B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{115BB8D9-8B86-4726-97F8-E06477FD353D}"/>
   </bookViews>
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="403">
   <si>
     <t>Lectura general</t>
   </si>
@@ -1195,15 +1195,6 @@
   </si>
   <si>
     <t>Currently, almost all of the DNN-based applications in seismic velocity inversion is to simplify the velocity models into some classes and then design an algorithm to generate enough velocity models for training the deep learning network. Thus, the generalization ability of the proposed deep learning inversion frameworks to a more complex velocity model would be an issue. One way to address this issue is to build or otherwise acquire a set of realistic velocity models which is of a larger scale and contain more complex structures such as salt bodies, faults, several different curved layers with different velocity distributions, etc. However, these kinds of improvements in the aspects of velocity model size and complexity are usually difficult, due to limitations of computation power such as memories, CPU, GPU and etc. Thus, the extension of current deep learning inversion philosophy to practical application may require extensive research work in the future.</t>
-  </si>
-  <si>
-    <t>Mixture Density Networks (MDNs)</t>
-  </si>
-  <si>
-    <t>we can also output uncertainties in the network</t>
-  </si>
-  <si>
-    <t>TensorFlow</t>
   </si>
   <si>
     <t>1. This is a research prototype since it develops and demonstrates new inversion and imaging methods (wavefield gradiometry, Helmholtz equation inversion and mixture density neural networks).
@@ -1325,18 +1316,6 @@
   </si>
   <si>
     <t> use several coupled deep neural networks to infer vary accuracy the velocity field.</t>
-  </si>
-  <si>
-    <t> Elastic-AdjointNet</t>
-  </si>
-  <si>
-    <t> a new network the input to which is the multicomponent shot gathers</t>
-  </si>
-  <si>
-    <t>We use the eighth-order staggered grid finite difference scheme in space and second order in time</t>
-  </si>
-  <si>
-    <t> Pytorch</t>
   </si>
   <si>
     <t> 1. This paper presents a research prototype that uses deep learning for seismic data processing.
@@ -1525,9 +1504,6 @@
 </t>
   </si>
   <si>
-    <t>Our framework needs no labelled training data nor pretraining of the network, is flexible to achieve multi-parameters inversion with minimal user interaction.</t>
-  </si>
-  <si>
     <t>It is worthy to note that in our work, we attempt to introduce a novel paradigm that integrating deep learning with physics equation to achieve the task of seismic inversion even when the conditions are difficult, instead of improving the conventional optimization algorithms for FWI. Therefore the comparisons with developed approaches such as multi-scale frequency inversion for FWI with l2 norm or other misfit function will be fixed in a future.</t>
   </si>
   <si>
@@ -1649,12 +1625,202 @@
   <si>
     <t>Synthetic data. Four datasets, of which three of them are used for seismic FWI, and one of which is for an EM inversion.</t>
   </si>
+  <si>
+    <t> 1) Research prototype
+2) Wave-equation traveltime (WT) inversion.
+Autoencoder-based feature extraction for seismic inversion.
+3) AE latent features remain sensitive to traveltime changes. Envelope + normalization preserves relevant refraction information. 
+4) Proposes elastic AEWT.
+5) Structure is clear: method, training, synthetic, field and discussion.</t>
+  </si>
+  <si>
+    <t>Autoencoder. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Improve the velocity tomography P when the data has a lot of noise, because it depends on picks or raw data, us a latent features automatically extracted by an autoencoder. </t>
+  </si>
+  <si>
+    <t> Finite difference.</t>
+  </si>
+  <si>
+    <t>  Not a public package; appears to be an in-house FD implementation.</t>
+  </si>
+  <si>
+    <t> Both synthetic and real data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2D </t>
+  </si>
+  <si>
+    <t>  Elastic.</t>
+  </si>
+  <si>
+    <t> The paper shows acoustic AEWT can fail in models with strong S-wave contributions (LVZ test), while elastic AEWT succeeds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Improved stability under noisy conditions.</t>
+  </si>
+  <si>
+    <t>Wave-equation traveltime inversion.</t>
+  </si>
+  <si>
+    <t>Visual comparison of tomograms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joint inversion of Vp and Vs simultaneously.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Not explicitly stated.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fourier Neural Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Learns a solution operator, not a single-case mapping and  fast inference.</t>
+  </si>
+  <si>
+    <t>Not explicitly stated.</t>
+  </si>
+  <si>
+    <t> Spectral element method</t>
+  </si>
+  <si>
+    <t>Not explicitly stated. </t>
+  </si>
+  <si>
+    <t>Synthetic data.</t>
+  </si>
+  <si>
+    <t>  2D</t>
+  </si>
+  <si>
+    <t> They claim the framework should extend to 3D elastic wave modeling with relatively little modification.</t>
+  </si>
+  <si>
+    <t>  They argue FNO has solved Navier–Stokes, suggesting elastic wave equations may be feasible.</t>
+  </si>
+  <si>
+    <t> SEM is used to generate training data.</t>
+  </si>
+  <si>
+    <t> Relative L2 loss.</t>
+  </si>
+  <si>
+    <t>Full waveform inversion.</t>
+  </si>
+  <si>
+    <t>1) Research prototype.
+2) Neural Operators and Teoría de operadores.
+3) Training on an ensemble of random velocity models and sources to learn a general solution operator.
+4)They explicitly note the solutions are approximate and performance depends on architecture, hyperparameters, and training data.
+5) The architecture and dataset generation are described clearly.</t>
+  </si>
+  <si>
+    <t>1) Research prototype
+2) Seismic While Drilling
+3) drill-string modeled as axial wave PDE with downhole boundary dynamics. The modeling assumptions are plausible for a controlled simulation study.
+4) A method to estimate force-on-bit and bit velocity using only surface measurements.
+5)  The paper is structured and the workflow is clear.</t>
+  </si>
+  <si>
+    <t> Multi-layer Perceptron regressor.</t>
+  </si>
+  <si>
+    <t> Fast inference once trained.</t>
+  </si>
+  <si>
+    <t>  scikit-learn</t>
+  </si>
+  <si>
+    <t> Yes, but not specified.</t>
+  </si>
+  <si>
+    <t>Synthetic data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1D </t>
+  </si>
+  <si>
+    <t>Not discussed. </t>
+  </si>
+  <si>
+    <t>Not disscused. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acoustic</t>
+  </si>
+  <si>
+    <t>ML is used as an alternative estimator. </t>
+  </si>
+  <si>
+    <t>Include axial–torsional coupling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Visual comparison plots.</t>
+  </si>
+  <si>
+    <t>Seismic-while-drilling to estimate formation properties.</t>
+  </si>
+  <si>
+    <t>1) Research prototype.
+2) Related to elastic multiparameter Full Waveform Inversión.
+3) Synthetic data generated by their forward solver and  limitations are mentioned indirectly (they focus on 2D, synthetic tests, and do not fully address field noise).
+4) Demonstrates reduction of crosstalk artifacts and improved performance in low illumination regions compared to conventional elastic FWI.
+5) The workflow is clearly described and supported by figures.</t>
+  </si>
+  <si>
+    <t>CNN-based encoder–decoder</t>
+  </si>
+  <si>
+    <t>PyTorch</t>
+  </si>
+  <si>
+    <t>Mitigate multiparameter crosstalk.</t>
+  </si>
+  <si>
+    <t> In-house solver</t>
+  </si>
+  <si>
+    <t>Finite differences</t>
+  </si>
+  <si>
+    <t>Synthetic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elastic</t>
+  </si>
+  <si>
+    <t> Affected by parameter coupling, which produces crosstalk.</t>
+  </si>
+  <si>
+    <t>  A standard PDE solver generates synthetic seismograms.</t>
+  </si>
+  <si>
+    <t> Elastic multiparameter Full Waveform Inversion</t>
+  </si>
+  <si>
+    <t>Use a variational autoencoder to support uncertainty quantification in multiparameter elastic FWI.</t>
+  </si>
+  <si>
+    <t>Misfit function based on L2 waveform difference and Comparison with conventional elastic FWI.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1704,6 +1870,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1725,7 +1903,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1764,11 +1942,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1876,11 +2065,18 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1893,6 +2089,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2328,7 +2527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA03A6B-77A3-4C70-96BD-6ED4FF8B301A}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2351,39 +2550,39 @@
   <sheetData>
     <row r="1" spans="1:16" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="40"/>
+      <c r="G1" s="43"/>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40" t="s">
+      <c r="J1" s="43"/>
+      <c r="K1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="40"/>
-      <c r="M1" s="41" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="42" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2391,7 +2590,7 @@
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
@@ -2422,10 +2621,10 @@
       <c r="L2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="39"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="42"/>
     </row>
     <row r="3" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -3328,7 +3527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86672D6-3E2B-4FF4-8D5A-4ACC029B5767}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -5439,10 +5638,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C33CE99-2E5D-4F6C-B637-1B3AEFE552A0}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5460,36 +5659,36 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="39"/>
+      <c r="G1" s="42"/>
       <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39" t="s">
+      <c r="J1" s="42"/>
+      <c r="K1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="42" t="s">
+      <c r="L1" s="42"/>
+      <c r="M1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="42" t="s">
+      <c r="N1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="O1" s="45" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5497,7 +5696,7 @@
       <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
@@ -5528,9 +5727,9 @@
       <c r="L2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
     </row>
     <row r="3" spans="1:15" ht="345" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -5763,7 +5962,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="360" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="375" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>26</v>
       </c>
@@ -6139,7 +6338,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="390" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="405" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>34</v>
       </c>
@@ -6164,8 +6363,8 @@
       <c r="H16" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="26">
-        <v>2</v>
+      <c r="I16" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="J16" s="26" t="s">
         <v>88</v>
@@ -6186,160 +6385,162 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:17" s="34" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="L17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="M17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="N17" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="O17" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="379.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>369</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>370</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="L17" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="M17" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="N17" s="33" t="s">
+        <v>374</v>
+      </c>
+      <c r="O17" s="33" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="379.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="F18" s="25" t="s">
         <v>247</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>250</v>
       </c>
       <c r="G18" s="24" t="s">
         <v>141</v>
       </c>
       <c r="H18" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="K18" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="L18" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="M18" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="K18" s="25" t="s">
+      <c r="N18" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="L18" s="25" t="s">
-        <v>255</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="N18" s="25" t="s">
-        <v>257</v>
-      </c>
       <c r="O18" s="26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="34" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="34" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="F19" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="G19" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="I19" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="J19" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="G19" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="H19" s="32" t="s">
+      <c r="K19" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="L19" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="M19" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="K19" s="32" t="s">
+      <c r="N19" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="L19" s="32" t="s">
+      <c r="O19" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="P19" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="M19" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="N19" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="O19" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="P19" s="35" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="409.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:17" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>141</v>
@@ -6353,11 +6554,11 @@
       <c r="H20" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="I20" s="26">
-        <v>2</v>
+      <c r="I20" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K20" s="22" t="s">
         <v>140</v>
@@ -6372,129 +6573,139 @@
         <v>88</v>
       </c>
       <c r="O20" s="30" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" s="34" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="K21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="L21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="M21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="N21" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="O21" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="B21" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>378</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="J21" s="33" t="s">
+        <v>383</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>385</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="M21" s="33" t="s">
+        <v>386</v>
+      </c>
+      <c r="N21" s="33" t="s">
+        <v>389</v>
+      </c>
+      <c r="O21" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="P21" s="34" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" s="34" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26" t="s">
-        <v>276</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>278</v>
-      </c>
-      <c r="G22" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="I22" s="26">
-        <v>2</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="M22" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="N22" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="O22" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="315" x14ac:dyDescent="0.25">
+      <c r="B22" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>393</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="K22" s="46" t="s">
+        <v>397</v>
+      </c>
+      <c r="L22" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="M22" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="O22" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>198</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="I23" s="26" t="s">
         <v>96</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="K23" s="22" t="s">
         <v>140</v>
@@ -6503,17 +6714,17 @@
         <v>88</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="N23" s="25"/>
       <c r="O23" s="25" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>42</v>
       </c>
@@ -6560,7 +6771,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>43</v>
       </c>
@@ -6607,30 +6818,30 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="330" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="330" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="F26" s="26" t="s">
         <v>148</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="I26" s="26" t="s">
         <v>109</v>
@@ -6649,10 +6860,10 @@
       </c>
       <c r="N26" s="25"/>
       <c r="O26" s="25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>45</v>
       </c>
@@ -6699,199 +6910,205 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="300" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="300" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="I28" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="J28" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="K28" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="L28" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="M28" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="N28" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="O28" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="I28" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="J28" s="25" t="s">
-        <v>303</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="L28" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="N28" s="25" t="s">
-        <v>307</v>
-      </c>
-      <c r="O28" s="25" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="34" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" s="34" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="I29" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="J29" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="K29" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="L29" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="M29" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="N29" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="O29" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="I29" s="32" t="s">
+      <c r="P29" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="J29" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>318</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="M29" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="N29" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="O29" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="P29" s="36" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="315" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+    </row>
+    <row r="30" spans="1:17" s="34" customFormat="1" ht="315" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="J30" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="K30" s="33" t="s">
         <v>342</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="L30" s="33" t="s">
         <v>343</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="M30" s="37" t="s">
         <v>344</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="N30" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="O30" s="33" t="s">
+        <v>347</v>
+      </c>
+      <c r="P30" s="35" t="s">
         <v>346</v>
       </c>
-      <c r="G30" s="26" t="s">
-        <v>347</v>
-      </c>
-      <c r="H30" s="26" t="s">
+    </row>
+    <row r="31" spans="1:17" s="34" customFormat="1" ht="180" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="K31" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="I30" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>349</v>
-      </c>
-      <c r="K30" s="26" t="s">
-        <v>350</v>
-      </c>
-      <c r="L30" s="26" t="s">
-        <v>351</v>
-      </c>
-      <c r="M30" s="37" t="s">
-        <v>352</v>
-      </c>
-      <c r="N30" s="25" t="s">
-        <v>353</v>
-      </c>
-      <c r="O30" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="P30" s="38" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="J31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="K31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="L31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="M31" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="N31" s="25" t="s">
-        <v>324</v>
-      </c>
-      <c r="O31" s="26"/>
-    </row>
-    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="L31" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="M31" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="O31" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="P31" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q31" s="39"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>50</v>
       </c>
@@ -6933,7 +7150,7 @@
       </c>
       <c r="N32" s="25"/>
       <c r="O32" s="26" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="390" x14ac:dyDescent="0.25">
@@ -6941,43 +7158,43 @@
         <v>51</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>141</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="J33" s="25" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="K33" s="26" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="L33" s="26" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="M33" s="25" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="O33" s="26"/>
     </row>
@@ -7023,7 +7240,7 @@
       </c>
       <c r="N34" s="25"/>
       <c r="O34" s="26" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -7067,7 +7284,7 @@
         <v>88</v>
       </c>
       <c r="N35" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="O35" s="26"/>
     </row>
@@ -7113,7 +7330,7 @@
       </c>
       <c r="N36" s="25"/>
       <c r="O36" s="26" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -7157,7 +7374,7 @@
         <v>88</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="O37" s="26" t="s">
         <v>88</v>
@@ -7249,7 +7466,7 @@
         <v>88</v>
       </c>
       <c r="N39" s="25" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="O39" s="26" t="s">
         <v>88</v>
@@ -7341,7 +7558,7 @@
         <v>88</v>
       </c>
       <c r="N41" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="O41" s="26" t="s">
         <v>88</v>

</xml_diff>